<commit_message>
updated spreadsheets with 2017+ changes
</commit_message>
<xml_diff>
--- a/rawdata/VZ_FederalMinimumWage_Changes.xlsx
+++ b/rawdata/VZ_FederalMinimumWage_Changes.xlsx
@@ -5,76 +5,81 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="564" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="982" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
-    <t>year</t>
-  </si>
-  <si>
-    <t>month</t>
-  </si>
-  <si>
-    <t>day</t>
-  </si>
-  <si>
-    <t>Fed_mw</t>
-  </si>
-  <si>
-    <t>source</t>
-  </si>
-  <si>
-    <t>Federal - DOL - Historical Minimum Wage Changes - 01.14.2016</t>
-  </si>
-  <si>
-    <t>Federal - DOL - Historical Minimum Wage Changes - 01.14.2017</t>
-  </si>
-  <si>
-    <t>Federal - DOL - Historical Minimum Wage Changes - 01.14.2018</t>
-  </si>
-  <si>
-    <t>Federal - DOL - Historical Minimum Wage Changes - 01.14.2019</t>
-  </si>
-  <si>
-    <t>Federal - DOL - Historical Minimum Wage Changes - 01.14.2020</t>
-  </si>
-  <si>
-    <t>Federal - DOL - Historical Minimum Wage Changes - 01.14.2021</t>
-  </si>
-  <si>
-    <t>Federal - DOL - Historical Minimum Wage Changes - 01.14.2022</t>
-  </si>
-  <si>
-    <t>Federal - DOL - Historical Minimum Wage Changes - 01.14.2023</t>
-  </si>
-  <si>
-    <t>Federal - DOL - Historical Minimum Wage Changes - 01.14.2024</t>
-  </si>
-  <si>
-    <t>Federal - DOL - Historical Minimum Wage Changes - 01.14.2025</t>
-  </si>
-  <si>
-    <t>Federal - DOL - Historical Minimum Wage Changes - 01.14.2026</t>
-  </si>
-  <si>
-    <t>Federal - DOL - Historical Minimum Wage Changes - 01.14.2027</t>
-  </si>
-  <si>
-    <t>Federal - DOL - Historical Minimum Wage Changes - 01.14.2028</t>
-  </si>
-  <si>
-    <t>Federal - DOL - Historical Minimum Wage Changes - 01.14.2029</t>
-  </si>
-  <si>
-    <t>CURRENT</t>
+    <t xml:space="preserve">year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">month</t>
+  </si>
+  <si>
+    <t xml:space="preserve">day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fed_mw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Federal - DOL - Historical Minimum Wage Changes - 01.14.2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Federal - DOL - Historical Minimum Wage Changes - 01.14.2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Federal - DOL - Historical Minimum Wage Changes - 01.14.2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Federal - DOL - Historical Minimum Wage Changes - 01.14.2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Federal - DOL - Historical Minimum Wage Changes - 01.14.2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Federal - DOL - Historical Minimum Wage Changes - 01.14.2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Federal - DOL - Historical Minimum Wage Changes - 01.14.2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Federal - DOL - Historical Minimum Wage Changes - 01.14.2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Federal - DOL - Historical Minimum Wage Changes - 01.14.2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Federal - DOL - Historical Minimum Wage Changes - 01.14.2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Federal - DOL - Historical Minimum Wage Changes - 01.14.2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Federal - DOL - Historical Minimum Wage Changes - 01.14.2027</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Federal - DOL - Historical Minimum Wage Changes - 01.14.2028</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Federal - DOL - Historical Minimum Wage Changes - 01.14.2029</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CURRENT</t>
   </si>
 </sst>
 </file>
@@ -82,7 +87,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -183,17 +188,17 @@
   <dimension ref="1:16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="1" width="18.668016194332"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.165991902834"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.502024291498"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.165991902834"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.502024291498"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.83400809716599"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="1" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.63775510204082"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -455,10 +460,10 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="B16" s="1" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C16" s="1" t="n">
         <v>1</v>

</xml_diff>